<commit_message>
Update zonal summaries and requirements.txt
</commit_message>
<xml_diff>
--- a/reports/zonal_distribution_resident_passengers.xlsx
+++ b/reports/zonal_distribution_resident_passengers.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,22 +442,32 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>num_travel_parties_non_synthetic</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>num_travel_parties_all</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>weighted_num_parties</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>num_travelers_non_synthetic</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>num_travelers_all</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>weighted_num_travelers</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>weighted_num_parties</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>num_travelers</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>num_travel_parties</t>
         </is>
       </c>
     </row>
@@ -468,16 +478,22 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>70</v>
+      </c>
+      <c r="C2" t="n">
+        <v>139</v>
+      </c>
+      <c r="D2" t="n">
+        <v>292.4885902952402</v>
+      </c>
+      <c r="E2" t="n">
+        <v>102</v>
+      </c>
+      <c r="F2" t="n">
+        <v>203</v>
+      </c>
+      <c r="G2" t="n">
         <v>526.8441995187937</v>
-      </c>
-      <c r="C2" t="n">
-        <v>292.4885902952402</v>
-      </c>
-      <c r="D2" t="n">
-        <v>102</v>
-      </c>
-      <c r="E2" t="n">
-        <v>70</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +503,22 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>102</v>
+      </c>
+      <c r="C3" t="n">
+        <v>202</v>
+      </c>
+      <c r="D3" t="n">
+        <v>711.3347177625194</v>
+      </c>
+      <c r="E3" t="n">
+        <v>187</v>
+      </c>
+      <c r="F3" t="n">
+        <v>370</v>
+      </c>
+      <c r="G3" t="n">
         <v>2361.19136066915</v>
-      </c>
-      <c r="C3" t="n">
-        <v>711.3347177625194</v>
-      </c>
-      <c r="D3" t="n">
-        <v>187</v>
-      </c>
-      <c r="E3" t="n">
-        <v>102</v>
       </c>
     </row>
     <row r="4">
@@ -506,16 +528,22 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>19</v>
+      </c>
+      <c r="C4" t="n">
+        <v>38</v>
+      </c>
+      <c r="D4" t="n">
+        <v>93.64261768814296</v>
+      </c>
+      <c r="E4" t="n">
+        <v>32</v>
+      </c>
+      <c r="F4" t="n">
+        <v>64</v>
+      </c>
+      <c r="G4" t="n">
         <v>213.0965688625636</v>
-      </c>
-      <c r="C4" t="n">
-        <v>93.64261768814296</v>
-      </c>
-      <c r="D4" t="n">
-        <v>32</v>
-      </c>
-      <c r="E4" t="n">
-        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -525,16 +553,22 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>13</v>
+      </c>
+      <c r="C5" t="n">
+        <v>26</v>
+      </c>
+      <c r="D5" t="n">
+        <v>51.84697728809346</v>
+      </c>
+      <c r="E5" t="n">
+        <v>18</v>
+      </c>
+      <c r="F5" t="n">
+        <v>36</v>
+      </c>
+      <c r="G5" t="n">
         <v>86.78637822663244</v>
-      </c>
-      <c r="C5" t="n">
-        <v>51.84697728809346</v>
-      </c>
-      <c r="D5" t="n">
-        <v>18</v>
-      </c>
-      <c r="E5" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -544,16 +578,22 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>39</v>
+      </c>
+      <c r="C6" t="n">
+        <v>75</v>
+      </c>
+      <c r="D6" t="n">
+        <v>194.9733874890915</v>
+      </c>
+      <c r="E6" t="n">
+        <v>70</v>
+      </c>
+      <c r="F6" t="n">
+        <v>135</v>
+      </c>
+      <c r="G6" t="n">
         <v>420.0230771500916</v>
-      </c>
-      <c r="C6" t="n">
-        <v>194.9733874890915</v>
-      </c>
-      <c r="D6" t="n">
-        <v>70</v>
-      </c>
-      <c r="E6" t="n">
-        <v>39</v>
       </c>
     </row>
     <row r="7">
@@ -563,16 +603,22 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>40</v>
+      </c>
+      <c r="C7" t="n">
+        <v>80</v>
+      </c>
+      <c r="D7" t="n">
+        <v>172.1939130706724</v>
+      </c>
+      <c r="E7" t="n">
+        <v>56</v>
+      </c>
+      <c r="F7" t="n">
+        <v>112</v>
+      </c>
+      <c r="G7" t="n">
         <v>374.6553754313406</v>
-      </c>
-      <c r="C7" t="n">
-        <v>172.1939130706724</v>
-      </c>
-      <c r="D7" t="n">
-        <v>56</v>
-      </c>
-      <c r="E7" t="n">
-        <v>40</v>
       </c>
     </row>
     <row r="8">
@@ -582,263 +628,347 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>43</v>
+      </c>
+      <c r="C8" t="n">
+        <v>86</v>
+      </c>
+      <c r="D8" t="n">
+        <v>338.4956636218766</v>
+      </c>
+      <c r="E8" t="n">
+        <v>80</v>
+      </c>
+      <c r="F8" t="n">
+        <v>160</v>
+      </c>
+      <c r="G8" t="n">
         <v>1177.077347882569</v>
-      </c>
-      <c r="C8" t="n">
-        <v>338.4956636218766</v>
-      </c>
-      <c r="D8" t="n">
-        <v>80</v>
-      </c>
-      <c r="E8" t="n">
-        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>EXTERNAL</t>
+          <t>IMPERIAL BEACH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3668.026532723073</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>1038.556966747412</v>
+        <v>16</v>
       </c>
       <c r="D9" t="n">
-        <v>309</v>
+        <v>28.3366914739767</v>
       </c>
       <c r="E9" t="n">
-        <v>156</v>
+        <v>10</v>
+      </c>
+      <c r="F9" t="n">
+        <v>20</v>
+      </c>
+      <c r="G9" t="n">
+        <v>38.01188183469321</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IMPERIAL BEACH</t>
+          <t>LA MESA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>38.01188183469321</v>
+        <v>30</v>
       </c>
       <c r="C10" t="n">
-        <v>28.3366914739767</v>
+        <v>59</v>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>116.5590052697882</v>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="F10" t="n">
+        <v>78</v>
+      </c>
+      <c r="G10" t="n">
+        <v>171.6480161049426</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LA MESA</t>
+          <t>LEMON GROVE</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>171.6480161049426</v>
+        <v>7</v>
       </c>
       <c r="C11" t="n">
-        <v>116.5590052697882</v>
+        <v>14</v>
       </c>
       <c r="D11" t="n">
-        <v>40</v>
+        <v>35.24575250742617</v>
       </c>
       <c r="E11" t="n">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="F11" t="n">
+        <v>22</v>
+      </c>
+      <c r="G11" t="n">
+        <v>63.00802359259052</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>LEMON GROVE</t>
+          <t>NATIONAL CITY</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>63.00802359259052</v>
+        <v>17</v>
       </c>
       <c r="C12" t="n">
-        <v>35.24575250742617</v>
+        <v>33</v>
       </c>
       <c r="D12" t="n">
-        <v>11</v>
+        <v>141.7173131862031</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>35</v>
+      </c>
+      <c r="F12" t="n">
+        <v>69</v>
+      </c>
+      <c r="G12" t="n">
+        <v>681.7801362904765</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>NATIONAL CITY</t>
+          <t>OCEANSIDE</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>681.7801362904765</v>
+        <v>64</v>
       </c>
       <c r="C13" t="n">
-        <v>141.7173131862031</v>
+        <v>125</v>
       </c>
       <c r="D13" t="n">
-        <v>35</v>
+        <v>292.8424057954805</v>
       </c>
       <c r="E13" t="n">
-        <v>17</v>
+        <v>88</v>
+      </c>
+      <c r="F13" t="n">
+        <v>172</v>
+      </c>
+      <c r="G13" t="n">
+        <v>593.5761476797395</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>OCEANSIDE</t>
+          <t>POWAY</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>593.5761476797395</v>
+        <v>25</v>
       </c>
       <c r="C14" t="n">
-        <v>292.8424057954805</v>
+        <v>49</v>
       </c>
       <c r="D14" t="n">
-        <v>88</v>
+        <v>108.4315070116118</v>
       </c>
       <c r="E14" t="n">
-        <v>64</v>
+        <v>37</v>
+      </c>
+      <c r="F14" t="n">
+        <v>73</v>
+      </c>
+      <c r="G14" t="n">
+        <v>188.6821424217474</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>POWAY</t>
+          <t>S.D. COUNTY</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>188.6821424217474</v>
+        <v>120</v>
       </c>
       <c r="C15" t="n">
-        <v>108.4315070116118</v>
+        <v>239</v>
       </c>
       <c r="D15" t="n">
-        <v>37</v>
+        <v>699.9445421634921</v>
       </c>
       <c r="E15" t="n">
-        <v>25</v>
+        <v>212</v>
+      </c>
+      <c r="F15" t="n">
+        <v>422</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2043.640348183798</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>S.D. COUNTY</t>
+          <t>SAN DIEGO</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2043.640348183798</v>
+        <v>797</v>
       </c>
       <c r="C16" t="n">
-        <v>699.9445421634921</v>
+        <v>1576</v>
       </c>
       <c r="D16" t="n">
-        <v>212</v>
+        <v>4012.763155759468</v>
       </c>
       <c r="E16" t="n">
-        <v>120</v>
+        <v>1244</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2465</v>
+      </c>
+      <c r="G16" t="n">
+        <v>9828.473771308905</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SAN DIEGO</t>
+          <t>SAN MARCOS</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>9828.473771308905</v>
+        <v>27</v>
       </c>
       <c r="C17" t="n">
-        <v>4012.763155759468</v>
+        <v>54</v>
       </c>
       <c r="D17" t="n">
-        <v>1244</v>
+        <v>164.8364240895055</v>
       </c>
       <c r="E17" t="n">
-        <v>797</v>
+        <v>47</v>
+      </c>
+      <c r="F17" t="n">
+        <v>94</v>
+      </c>
+      <c r="G17" t="n">
+        <v>527.4339953915301</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SAN MARCOS</t>
+          <t>SANTEE</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>527.4339953915301</v>
+        <v>9</v>
       </c>
       <c r="C18" t="n">
-        <v>164.8364240895055</v>
+        <v>18</v>
       </c>
       <c r="D18" t="n">
-        <v>47</v>
+        <v>43.98416920614759</v>
       </c>
       <c r="E18" t="n">
-        <v>27</v>
+        <v>13</v>
+      </c>
+      <c r="F18" t="n">
+        <v>26</v>
+      </c>
+      <c r="G18" t="n">
+        <v>84.95431503120587</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SANTEE</t>
+          <t>SOLANA BEACH</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>84.95431503120587</v>
+        <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>43.98416920614759</v>
+        <v>12</v>
       </c>
       <c r="D19" t="n">
-        <v>13</v>
+        <v>27.73569131627352</v>
       </c>
       <c r="E19" t="n">
         <v>9</v>
       </c>
+      <c r="F19" t="n">
+        <v>18</v>
+      </c>
+      <c r="G19" t="n">
+        <v>45.28465470270577</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SOLANA BEACH</t>
+          <t>VISTA</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>45.28465470270577</v>
+        <v>12</v>
       </c>
       <c r="C20" t="n">
-        <v>27.73569131627352</v>
+        <v>24</v>
       </c>
       <c r="D20" t="n">
-        <v>9</v>
+        <v>64.61316482390929</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="F20" t="n">
+        <v>44</v>
+      </c>
+      <c r="G20" t="n">
+        <v>171.8938651302715</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>VISTA</t>
+          <t>EXTERNAL</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>171.8938651302715</v>
+        <v>156</v>
       </c>
       <c r="C21" t="n">
-        <v>64.61316482390929</v>
+        <v>305</v>
       </c>
       <c r="D21" t="n">
-        <v>22</v>
+        <v>1038.556966747412</v>
       </c>
       <c r="E21" t="n">
-        <v>12</v>
+        <v>309</v>
+      </c>
+      <c r="F21" t="n">
+        <v>608</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3668.026532723073</v>
       </c>
     </row>
   </sheetData>
@@ -852,7 +982,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -868,22 +998,32 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>num_travel_parties_non_synthetic</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>num_travel_parties_all</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>weighted_num_parties</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>num_travelers_non_synthetic</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>num_travelers_all</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>weighted_num_travelers</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>weighted_num_parties</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>num_travelers</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>num_travel_parties</t>
         </is>
       </c>
     </row>
@@ -892,16 +1032,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
+        <v>62</v>
+      </c>
+      <c r="C2" t="n">
+        <v>124</v>
+      </c>
+      <c r="D2" t="n">
+        <v>428.0549411780708</v>
+      </c>
+      <c r="E2" t="n">
+        <v>105</v>
+      </c>
+      <c r="F2" t="n">
+        <v>210</v>
+      </c>
+      <c r="G2" t="n">
         <v>1427.068212755847</v>
-      </c>
-      <c r="C2" t="n">
-        <v>428.0549411780708</v>
-      </c>
-      <c r="D2" t="n">
-        <v>105</v>
-      </c>
-      <c r="E2" t="n">
-        <v>62</v>
       </c>
     </row>
     <row r="3">
@@ -909,16 +1055,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
+        <v>350</v>
+      </c>
+      <c r="C3" t="n">
+        <v>689</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1814.357443196731</v>
+      </c>
+      <c r="E3" t="n">
+        <v>565</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1116</v>
+      </c>
+      <c r="G3" t="n">
         <v>4579.221813028876</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1814.357443196731</v>
-      </c>
-      <c r="D3" t="n">
-        <v>565</v>
-      </c>
-      <c r="E3" t="n">
-        <v>350</v>
       </c>
     </row>
     <row r="4">
@@ -926,16 +1078,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
+        <v>444</v>
+      </c>
+      <c r="C4" t="n">
+        <v>879</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2133.674078262204</v>
+      </c>
+      <c r="E4" t="n">
+        <v>685</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1359</v>
+      </c>
+      <c r="G4" t="n">
         <v>5010.17304689853</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2133.674078262204</v>
-      </c>
-      <c r="D4" t="n">
-        <v>685</v>
-      </c>
-      <c r="E4" t="n">
-        <v>444</v>
       </c>
     </row>
     <row r="5">
@@ -943,16 +1101,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
+        <v>130</v>
+      </c>
+      <c r="C5" t="n">
+        <v>258</v>
+      </c>
+      <c r="D5" t="n">
+        <v>816.7752897589887</v>
+      </c>
+      <c r="E5" t="n">
+        <v>223</v>
+      </c>
+      <c r="F5" t="n">
+        <v>442</v>
+      </c>
+      <c r="G5" t="n">
         <v>2512.470793619224</v>
-      </c>
-      <c r="C5" t="n">
-        <v>816.7752897589887</v>
-      </c>
-      <c r="D5" t="n">
-        <v>223</v>
-      </c>
-      <c r="E5" t="n">
-        <v>130</v>
       </c>
     </row>
     <row r="6">
@@ -960,16 +1124,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
+        <v>148</v>
+      </c>
+      <c r="C6" t="n">
+        <v>292</v>
+      </c>
+      <c r="D6" t="n">
+        <v>767.6735760273507</v>
+      </c>
+      <c r="E6" t="n">
+        <v>246</v>
+      </c>
+      <c r="F6" t="n">
+        <v>485</v>
+      </c>
+      <c r="G6" t="n">
         <v>1949.73505025599</v>
-      </c>
-      <c r="C6" t="n">
-        <v>767.6735760273507</v>
-      </c>
-      <c r="D6" t="n">
-        <v>246</v>
-      </c>
-      <c r="E6" t="n">
-        <v>148</v>
       </c>
     </row>
     <row r="7">
@@ -977,16 +1147,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
+        <v>209</v>
+      </c>
+      <c r="C7" t="n">
+        <v>413</v>
+      </c>
+      <c r="D7" t="n">
+        <v>900.9134211179203</v>
+      </c>
+      <c r="E7" t="n">
+        <v>294</v>
+      </c>
+      <c r="F7" t="n">
+        <v>581</v>
+      </c>
+      <c r="G7" t="n">
         <v>1756.762086194048</v>
-      </c>
-      <c r="C7" t="n">
-        <v>900.9134211179203</v>
-      </c>
-      <c r="D7" t="n">
-        <v>294</v>
-      </c>
-      <c r="E7" t="n">
-        <v>209</v>
       </c>
     </row>
     <row r="8">
@@ -994,16 +1170,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
+        <v>101</v>
+      </c>
+      <c r="C8" t="n">
+        <v>202</v>
+      </c>
+      <c r="D8" t="n">
+        <v>704.702734615641</v>
+      </c>
+      <c r="E8" t="n">
+        <v>189</v>
+      </c>
+      <c r="F8" t="n">
+        <v>378</v>
+      </c>
+      <c r="G8" t="n">
         <v>2305.501441534878</v>
-      </c>
-      <c r="C8" t="n">
-        <v>704.702734615641</v>
-      </c>
-      <c r="D8" t="n">
-        <v>189</v>
-      </c>
-      <c r="E8" t="n">
-        <v>101</v>
       </c>
     </row>
     <row r="9">
@@ -1011,16 +1193,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>25.83420566201216</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F9" t="n">
+        <v>12</v>
+      </c>
+      <c r="G9" t="n">
         <v>57.12916112635393</v>
-      </c>
-      <c r="C9" t="n">
-        <v>25.83420566201216</v>
-      </c>
-      <c r="D9" t="n">
-        <v>6</v>
-      </c>
-      <c r="E9" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -1028,16 +1216,22 @@
         <v>99</v>
       </c>
       <c r="B10" t="n">
+        <v>156</v>
+      </c>
+      <c r="C10" t="n">
+        <v>305</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1038.556966747412</v>
+      </c>
+      <c r="E10" t="n">
+        <v>309</v>
+      </c>
+      <c r="F10" t="n">
+        <v>608</v>
+      </c>
+      <c r="G10" t="n">
         <v>3668.026532723073</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1038.556966747412</v>
-      </c>
-      <c r="D10" t="n">
-        <v>309</v>
-      </c>
-      <c r="E10" t="n">
-        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>